<commit_message>
Excel file includes new columns.
</commit_message>
<xml_diff>
--- a/metadata_ddl/Excel/turbovault4dbt_template.xlsx
+++ b/metadata_ddl/Excel/turbovault4dbt_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20404"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoffmann\Documents\VSC\Turbovault4dbt\turbovault4dbt\metadata_ddl\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\e720170\PycharmProjects\pythonProject\dbt-env\turbovault4dbt\metadata_ddl\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{902B4625-A9B0-4313-B6A8-E1D5E2E64905}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69DE645D-1989-4231-A644-F4075A6A3EB8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="38625" windowHeight="21105" tabRatio="792" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="standard_hub" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="47">
   <si>
     <t>Hub_Identifier</t>
   </si>
@@ -159,6 +159,15 @@
   </si>
   <si>
     <t>NH_Satellite_Identifier</t>
+  </si>
+  <si>
+    <t>Record_Tracking_Satellite</t>
+  </si>
+  <si>
+    <t>Is_Primary_Source</t>
+  </si>
+  <si>
+    <t>Group_Name</t>
   </si>
 </sst>
 </file>
@@ -187,11 +196,6 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFF0000"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -225,6 +229,13 @@
       <i/>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -269,29 +280,27 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="4" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -507,47 +516,59 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.90625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="32.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:10" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="H1" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -555,8 +576,9 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="J2" s="5"/>
+    </row>
+    <row r="3" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -564,8 +586,9 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="J3" s="5"/>
+    </row>
+    <row r="4" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -573,8 +596,9 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-    </row>
-    <row r="5" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="J4" s="5"/>
+    </row>
+    <row r="5" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -582,8 +606,9 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="J5" s="5"/>
+    </row>
+    <row r="6" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -591,8 +616,9 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="J6" s="5"/>
+    </row>
+    <row r="7" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -600,8 +626,9 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="J7" s="5"/>
+    </row>
+    <row r="8" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -609,8 +636,9 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="J8" s="5"/>
+    </row>
+    <row r="9" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -619,7 +647,7 @@
       <c r="F9" s="3"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -628,7 +656,7 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -639,6 +667,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -647,92 +676,97 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:M1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:O13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="28.90625" customWidth="1"/>
-    <col min="3" max="3" width="21.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.90625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="27.81640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24.90625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="32.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:15" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="L1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="M1" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
+      <c r="N1" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C2" s="1"/>
-      <c r="D2" s="2"/>
+      <c r="D2" s="1"/>
+      <c r="F2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
-    </row>
-    <row r="3" spans="1:13" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
+      <c r="O2" s="5"/>
+    </row>
+    <row r="3" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
       <c r="M3" s="1"/>
-    </row>
-    <row r="4" spans="1:13" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="O3" s="5"/>
+    </row>
+    <row r="4" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -743,7 +777,7 @@
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
     </row>
-    <row r="5" spans="1:13" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -754,7 +788,7 @@
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
     </row>
-    <row r="6" spans="1:13" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -765,7 +799,7 @@
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
     </row>
-    <row r="7" spans="1:13" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -786,112 +820,121 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:H1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.08984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.36328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="9" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="I1" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
-      <c r="B2" s="2"/>
+      <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
-    </row>
-    <row r="3" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="I2" s="5"/>
+    </row>
+    <row r="3" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
-      <c r="B3" s="2"/>
+      <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="I3" s="5"/>
+    </row>
+    <row r="4" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
-      <c r="B4" s="2"/>
+      <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="I4" s="5"/>
+    </row>
+    <row r="5" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
-      <c r="B5" s="2"/>
+      <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="I5" s="5"/>
+    </row>
+    <row r="6" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
-      <c r="B6" s="2"/>
+      <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="I6" s="5"/>
+    </row>
+    <row r="7" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
-      <c r="B7" s="2"/>
+      <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
-    </row>
-    <row r="8" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="I7" s="5"/>
+    </row>
+    <row r="8" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="C8" s="1"/>
@@ -901,7 +944,7 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="C9" s="1"/>
@@ -911,7 +954,7 @@
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="C10" s="1"/>
@@ -921,7 +964,7 @@
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="C11" s="1"/>
@@ -931,7 +974,7 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="C12" s="1"/>
@@ -941,7 +984,7 @@
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="C13" s="1"/>
@@ -951,7 +994,7 @@
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="C14" s="1"/>
@@ -961,7 +1004,7 @@
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
       <c r="C15" s="1"/>
@@ -971,7 +1014,7 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="C16" s="1"/>
@@ -981,7 +1024,7 @@
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="C17" s="1"/>
@@ -991,7 +1034,7 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
       <c r="C18" s="1"/>
@@ -1001,7 +1044,7 @@
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
       <c r="C19" s="1"/>
@@ -1011,7 +1054,7 @@
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
     </row>
-    <row r="20" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
       <c r="C20" s="1"/>
@@ -1021,7 +1064,7 @@
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
     </row>
-    <row r="21" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
       <c r="C21" s="1"/>
@@ -1031,7 +1074,7 @@
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
     </row>
-    <row r="22" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
       <c r="C22" s="1"/>
@@ -1041,7 +1084,7 @@
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1051,7 +1094,7 @@
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
     </row>
-    <row r="24" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1063,6 +1106,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1071,55 +1115,58 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:I1"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.08984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.90625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="10" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="J1" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="1"/>
@@ -1130,7 +1177,7 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="C3" s="1"/>
@@ -1141,7 +1188,7 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
       <c r="C4" s="1"/>
@@ -1152,46 +1199,46 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B10" s="2"/>
     </row>
-    <row r="11" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B12" s="2"/>
     </row>
-    <row r="13" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B13" s="2"/>
     </row>
-    <row r="14" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B14" s="2"/>
     </row>
-    <row r="15" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B15" s="2"/>
     </row>
-    <row r="16" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B16" s="2"/>
     </row>
-    <row r="17" spans="2:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B17" s="2"/>
     </row>
-    <row r="18" spans="2:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B18" s="2"/>
     </row>
   </sheetData>
@@ -1204,114 +1251,120 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:M1"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="30" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="27.81640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24.90625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="32.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="32.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:15" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="L1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="M1" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="N1" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
-      <c r="B2" s="5"/>
+      <c r="B2" s="4"/>
       <c r="C2" s="1"/>
       <c r="D2" s="2"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
-      <c r="M2" s="5"/>
-    </row>
-    <row r="3" spans="1:13" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="M2" s="4"/>
+    </row>
+    <row r="3" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
-      <c r="B3" s="5"/>
+      <c r="B3" s="4"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
-      <c r="M3" s="5"/>
-    </row>
-    <row r="4" spans="1:13" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="M3" s="4"/>
+    </row>
+    <row r="4" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
-      <c r="B4" s="5"/>
+      <c r="B4" s="4"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:13" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
-      <c r="B5" s="5"/>
+      <c r="B5" s="4"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:13" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="B6" s="5"/>
-    </row>
-    <row r="7" spans="1:13" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="B7" s="5"/>
-    </row>
-    <row r="8" spans="1:13" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="B8" s="5"/>
+    <row r="6" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B6" s="4"/>
+    </row>
+    <row r="7" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B7" s="4"/>
+    </row>
+    <row r="8" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B8" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1324,47 +1377,50 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G1"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.08984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="43" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:8" ht="42.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="9" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H1" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="1"/>
@@ -1373,7 +1429,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="C3" s="1"/>
@@ -1382,7 +1438,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
       <c r="C4" s="1"/>
@@ -1391,7 +1447,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
       <c r="C5" s="1"/>
@@ -1400,7 +1456,7 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="C6" s="1"/>
@@ -1409,7 +1465,7 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="C7" s="1"/>
@@ -1418,7 +1474,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="C8" s="1"/>
@@ -1427,7 +1483,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="C9" s="1"/>
@@ -1436,7 +1492,7 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="C10" s="1"/>
@@ -1445,7 +1501,7 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="C11" s="1"/>
@@ -1454,7 +1510,7 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="C12" s="1"/>
@@ -1463,7 +1519,7 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="C13" s="1"/>
@@ -1472,7 +1528,7 @@
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="C14" s="1"/>
@@ -1481,7 +1537,7 @@
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
       <c r="C15" s="1"/>
@@ -1490,7 +1546,7 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="C16" s="1"/>
@@ -1509,51 +1565,58 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="A1:G1"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="13" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H1" s="13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1565,111 +1628,119 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.36328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="33.08984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="11" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I1" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-    </row>
-    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F2" s="1"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="15"/>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-    </row>
-    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F3" s="1"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="15"/>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="15"/>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-    </row>
-    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="15"/>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="7"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
comments, primary key constraints, foreign key constraints
</commit_message>
<xml_diff>
--- a/metadata_ddl/Excel/turbovault4dbt_template.xlsx
+++ b/metadata_ddl/Excel/turbovault4dbt_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\software\datavaultstarter\turbovault4dbt\metadata_ddl\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A71A8689-1D96-4A6A-948F-EEFA6EFCFC89}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07D1E0D0-D25F-4F3C-8D9D-CB9B80F6EEF2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="38625" windowHeight="21105" tabRatio="792" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -525,9 +525,7 @@
   </sheetPr>
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>